<commit_message>
AutoCommit_29 сентября 2023 г. 10:05:57_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -509,10 +509,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -668,8 +668,12 @@
       <c r="D11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_6 октября 2023 г. 9:40:05_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>ок</t>
+  </si>
+  <si>
+    <t>д5</t>
+  </si>
+  <si>
+    <t>д6</t>
   </si>
 </sst>
 </file>
@@ -512,7 +518,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -560,8 +566,12 @@
       <c r="F3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4" spans="1:23" ht="13" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
@@ -674,8 +684,12 @@
       <c r="F11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="1:23" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">

</xml_diff>

<commit_message>
AutoCommit_6 октября 2023 г. 10:17:20_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -515,10 +515,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -759,7 +759,9 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">

</xml_diff>

<commit_message>
AutoCommit_6 октября 2023 г. 10:20:34_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -518,7 +518,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -840,7 +840,9 @@
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_6 октября 2023 г. 10:41:55_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -515,10 +515,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -649,7 +649,9 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" spans="1:23" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">

</xml_diff>

<commit_message>
AutoCommit_12 октября 2023 г. 13:52:49_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -518,7 +518,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -644,11 +644,21 @@
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="H9" s="2" t="s">
         <v>34</v>
       </c>
@@ -758,9 +768,15 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="H16" s="2" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_20 октября 2023 г. 9:11:38_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -515,10 +515,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -863,11 +863,17 @@
       <c r="C22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="23" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -994,10 +1000,18 @@
       <c r="D31" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">

</xml_diff>

<commit_message>
AutoCommit_23 октября 2023 г. 10:16:58_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -866,8 +866,12 @@
       <c r="D22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="G22" s="2" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_2 ноября 2023 г. 13:51:20_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -515,10 +515,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -639,7 +639,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -665,7 +665,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -678,8 +678,11 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="I10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -754,14 +757,24 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="E15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -783,21 +796,36 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -811,7 +839,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -825,7 +853,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -839,7 +867,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -865,7 +893,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -891,7 +919,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -905,21 +933,36 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="C24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -933,7 +976,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -947,7 +990,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -961,7 +1004,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -975,7 +1018,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -989,7 +1032,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -1003,7 +1046,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -1029,7 +1072,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_3 ноября 2023 г. 10:12:05_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -518,7 +518,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17:I17"/>
+      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -750,7 +750,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -793,6 +793,9 @@
         <v>34</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -853,7 +856,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -867,7 +870,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -892,8 +895,11 @@
       <c r="H21" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="I21" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_9 ноября 2023 г. 13:40:21_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -518,7 +518,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -739,10 +739,18 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" spans="1:23" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">

</xml_diff>

<commit_message>
AutoCommit_9 ноября 2023 г. 13:44:17_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -515,10 +515,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -959,6 +959,9 @@
       <c r="H22" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="I22" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
@@ -1136,11 +1139,17 @@
       <c r="B33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="G33" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_9 ноября 2023 г. 15:51:27_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -515,10 +515,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G33" sqref="G33"/>
+      <selection pane="bottomRight" activeCell="C30" sqref="C30:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1085,10 +1085,18 @@
       <c r="B30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_10 ноября 2023 г. 10:38:51_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -136,7 +136,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -158,6 +158,21 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -195,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -208,6 +223,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -515,10 +536,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C30" sqref="C30:F30"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -710,7 +731,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -730,15 +751,19 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E13" s="2" t="s">
         <v>34</v>
       </c>
@@ -751,8 +776,11 @@
       <c r="H13" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="I13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -855,12 +883,24 @@
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -1174,5 +1214,6 @@
     <mergeCell ref="C1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AutoCommit_10 ноября 2023 г. 10:39:32_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -221,14 +221,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -539,7 +539,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -550,29 +550,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
     </row>
     <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -602,7 +602,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -618,21 +618,36 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -886,7 +901,7 @@
       <c r="C18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -895,7 +910,7 @@
       <c r="F18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="5" t="s">
         <v>34</v>
       </c>
       <c r="H18" s="2" t="s">

</xml_diff>

<commit_message>
AutoCommit_10 ноября 2023 г. 10:42:51_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -539,7 +539,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomRight" activeCell="C19" sqref="C19:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -924,12 +924,27 @@
       <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">

</xml_diff>

<commit_message>
AutoCommit_10 ноября 2023 г. 11:27:34_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -539,7 +539,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C19" sqref="C19:I19"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -654,14 +654,27 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="H7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -1090,33 +1103,58 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="C26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">

</xml_diff>

<commit_message>
AutoCommit_10 ноября 2023 г. 11:28:49_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -536,10 +536,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1096,12 +1096,22 @@
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="F25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">

</xml_diff>

<commit_message>
AutoCommit_10 ноября 2023 г. 11:29:58_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -536,10 +536,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -715,6 +715,10 @@
       <c r="H9" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="I9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">

</xml_diff>

<commit_message>
AutoCommit_24 ноября 2023 г. 11:46:06_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -180,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -203,11 +203,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -227,6 +238,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -533,11 +547,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O14" sqref="O14"/>
+      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -760,18 +774,30 @@
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="C10" s="2">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
       <c r="I10" s="2">
         <v>5</v>
       </c>
       <c r="K10" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="M10">
         <v>3</v>
@@ -1166,9 +1192,12 @@
       <c r="I22" s="2">
         <v>5</v>
       </c>
+      <c r="J22" s="9">
+        <v>5</v>
+      </c>
       <c r="K22" s="6">
-        <f t="shared" si="0"/>
-        <v>35</v>
+        <f>SUM(C22:J22)</f>
+        <v>40</v>
       </c>
       <c r="M22">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_30 ноября 2023 г. 13:52:44_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -236,11 +236,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -548,10 +548,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
+      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -562,29 +562,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -795,9 +795,12 @@
       <c r="I10" s="2">
         <v>5</v>
       </c>
+      <c r="J10" s="7">
+        <v>5</v>
+      </c>
       <c r="K10" s="6">
-        <f t="shared" si="0"/>
-        <v>35</v>
+        <f>SUM(C10:J10)</f>
+        <v>40</v>
       </c>
       <c r="M10">
         <v>3</v>
@@ -1192,7 +1195,7 @@
       <c r="I22" s="2">
         <v>5</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22" s="7">
         <v>5</v>
       </c>
       <c r="K22" s="6">
@@ -1212,13 +1215,20 @@
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2">
+        <v>5</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="H23" s="2">
+        <v>5</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
       <c r="K23" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M23">
         <v>2</v>
@@ -1471,15 +1481,25 @@
       <c r="B32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="C32" s="2">
+        <v>5</v>
+      </c>
+      <c r="D32" s="2">
+        <v>5</v>
+      </c>
+      <c r="E32" s="2">
+        <v>5</v>
+      </c>
+      <c r="F32" s="2">
+        <v>5</v>
+      </c>
+      <c r="G32" s="2">
+        <v>5</v>
+      </c>
       <c r="H32" s="2"/>
       <c r="K32" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M32">
         <v>2</v>

</xml_diff>

<commit_message>
AutoCommit_7 декабря 2023 г. 12:39:46_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>2ИСИП-522: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>д6</t>
+  </si>
+  <si>
+    <t>д7</t>
+  </si>
+  <si>
+    <t>д8</t>
+  </si>
+  <si>
+    <t>д9</t>
   </si>
 </sst>
 </file>
@@ -248,11 +257,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -560,10 +569,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomRight" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -574,31 +583,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-    </row>
-    <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+    </row>
+    <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
@@ -617,8 +627,17 @@
       <c r="H3" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="I3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -641,13 +660,6 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="K5">
-        <f>SUM(C5:I5)</f>
-        <v>5</v>
-      </c>
-      <c r="M5">
-        <v>3</v>
-      </c>
     </row>
     <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -677,13 +689,7 @@
       <c r="I6" s="2">
         <v>5</v>
       </c>
-      <c r="K6" s="6">
-        <f t="shared" ref="K6:K33" si="0">SUM(C6:I6)</f>
-        <v>35</v>
-      </c>
-      <c r="M6">
-        <v>5</v>
-      </c>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -711,13 +717,7 @@
       <c r="I7" s="2">
         <v>5</v>
       </c>
-      <c r="K7" s="6">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="M7">
-        <v>5</v>
-      </c>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -734,13 +734,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="K8" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="M8">
-        <v>3</v>
-      </c>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -771,13 +765,7 @@
         <v>5</v>
       </c>
       <c r="J9" s="2"/>
-      <c r="K9" s="6">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M9">
-        <v>5</v>
-      </c>
+      <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -810,13 +798,7 @@
       <c r="J10" s="7">
         <v>5</v>
       </c>
-      <c r="K10" s="6">
-        <f>SUM(C10:J10)</f>
-        <v>40</v>
-      </c>
-      <c r="M10">
-        <v>3</v>
-      </c>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -843,17 +825,13 @@
       <c r="H11" s="2">
         <v>5</v>
       </c>
-      <c r="I11" s="10">
-        <v>5</v>
-      </c>
-      <c r="J11" s="10">
-        <v>5</v>
-      </c>
-      <c r="K11" s="6">
-        <f>SUM(C11:J11)</f>
-        <v>40</v>
-      </c>
-      <c r="M11">
+      <c r="I11" s="8">
+        <v>5</v>
+      </c>
+      <c r="J11" s="8">
+        <v>5</v>
+      </c>
+      <c r="K11" s="8">
         <v>5</v>
       </c>
     </row>
@@ -876,13 +854,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="K12" s="6">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="M12">
-        <v>4</v>
-      </c>
+      <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -912,13 +884,7 @@
       <c r="I13" s="2">
         <v>5</v>
       </c>
-      <c r="K13" s="6">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M13">
-        <v>5</v>
-      </c>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -927,19 +893,31 @@
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="K14" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>3</v>
-      </c>
+      <c r="C14" s="2">
+        <v>5</v>
+      </c>
+      <c r="D14" s="2">
+        <v>5</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14" s="2">
+        <v>5</v>
+      </c>
+      <c r="G14" s="2">
+        <v>5</v>
+      </c>
+      <c r="H14" s="2">
+        <v>5</v>
+      </c>
+      <c r="I14" s="8">
+        <v>5</v>
+      </c>
+      <c r="J14" s="8">
+        <v>5</v>
+      </c>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -964,13 +942,7 @@
       <c r="H15" s="2">
         <v>5</v>
       </c>
-      <c r="K15" s="6">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="M15">
-        <v>5</v>
-      </c>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -1003,15 +975,9 @@
       <c r="J16" s="7">
         <v>5</v>
       </c>
-      <c r="K16" s="6">
-        <f>SUM(C16:J16)</f>
-        <v>40</v>
-      </c>
-      <c r="M16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -1039,15 +1005,9 @@
       <c r="I17" s="2">
         <v>5</v>
       </c>
-      <c r="K17" s="6">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -1072,15 +1032,9 @@
       <c r="H18" s="2">
         <v>5</v>
       </c>
-      <c r="K18" s="6">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="M18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -1108,15 +1062,9 @@
       <c r="I19" s="2">
         <v>5</v>
       </c>
-      <c r="K19" s="6">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -1144,15 +1092,14 @@
       <c r="I20" s="2">
         <v>5</v>
       </c>
-      <c r="K20" s="6">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J20" s="7">
+        <v>5</v>
+      </c>
+      <c r="K20" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -1180,15 +1127,9 @@
       <c r="I21" s="2">
         <v>5</v>
       </c>
-      <c r="K21" s="6">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -1219,23 +1160,21 @@
       <c r="J22" s="7">
         <v>5</v>
       </c>
-      <c r="K22" s="6">
-        <f>SUM(C22:J22)</f>
-        <v>40</v>
-      </c>
-      <c r="M22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="C23" s="2">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2">
+        <v>5</v>
+      </c>
       <c r="E23" s="2">
         <v>5</v>
       </c>
@@ -1249,15 +1188,9 @@
       <c r="J23">
         <v>5</v>
       </c>
-      <c r="K23" s="6">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="M23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -1285,15 +1218,14 @@
       <c r="I24" s="2">
         <v>5</v>
       </c>
-      <c r="K24" s="6">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" s="7">
+        <v>5</v>
+      </c>
+      <c r="K24" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -1316,15 +1248,9 @@
       <c r="H25" s="2">
         <v>5</v>
       </c>
-      <c r="K25" s="6">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="M25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -1352,15 +1278,9 @@
       <c r="I26" s="2">
         <v>5</v>
       </c>
-      <c r="K26" s="6">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -1383,15 +1303,9 @@
       <c r="H27" s="2">
         <v>5</v>
       </c>
-      <c r="K27" s="6">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="M27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -1404,15 +1318,9 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="K28" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -1427,15 +1335,9 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="K29" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="M29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -1454,17 +1356,15 @@
       <c r="F30" s="2">
         <v>5</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="K30" s="6">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="M30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="G30" s="2">
+        <v>5</v>
+      </c>
+      <c r="H30" s="2">
+        <v>5</v>
+      </c>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -1489,15 +1389,9 @@
       <c r="H31" s="2">
         <v>5</v>
       </c>
-      <c r="K31" s="6">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="M31">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="K31" s="6"/>
+    </row>
+    <row r="32" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -1520,15 +1414,9 @@
         <v>5</v>
       </c>
       <c r="H32" s="2"/>
-      <c r="K32" s="6">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="M32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="K32" s="6"/>
+    </row>
+    <row r="33" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -1556,15 +1444,9 @@
       <c r="I33" s="7">
         <v>5</v>
       </c>
-      <c r="K33" s="6">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M33">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K33" s="6"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -1577,30 +1459,6 @@
   <mergeCells count="1">
     <mergeCell ref="C1:W1"/>
   </mergeCells>
-  <conditionalFormatting sqref="K5:K33">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M5:M33">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
AutoCommit_7 декабря 2023 г. 13:33:03_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -578,10 +578,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M27" sqref="M27"/>
+      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -747,14 +747,20 @@
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2">
+        <v>5</v>
+      </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
         <v>5</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
       <c r="K8" s="6"/>
       <c r="M8">
         <v>1</v>
@@ -1105,6 +1111,9 @@
         <v>5</v>
       </c>
       <c r="K19" s="6"/>
+      <c r="M19">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">

</xml_diff>

<commit_message>
AutoCommit_7 декабря 2023 г. 13:37:47_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -581,7 +581,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -796,6 +796,9 @@
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="6"/>
+      <c r="M9">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -1373,6 +1376,9 @@
         <v>5</v>
       </c>
       <c r="H27" s="2">
+        <v>5</v>
+      </c>
+      <c r="I27" s="7">
         <v>5</v>
       </c>
       <c r="K27" s="6"/>

</xml_diff>

<commit_message>
AutoCommit_8 декабря 2023 г. 10:25:16_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -582,7 +582,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -679,7 +679,7 @@
       </c>
       <c r="P4" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q4" s="11">
         <f t="shared" si="0"/>
@@ -947,6 +947,9 @@
         <v>5</v>
       </c>
       <c r="K10" s="6"/>
+      <c r="M10" s="10">
+        <v>3</v>
+      </c>
       <c r="N10" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -957,7 +960,7 @@
       </c>
       <c r="P10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="11">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
AutoCommit_8 декабря 2023 г. 11:09:30_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -582,7 +582,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -893,8 +893,12 @@
       <c r="I9" s="2">
         <v>5</v>
       </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="6"/>
+      <c r="J9" s="2">
+        <v>5</v>
+      </c>
+      <c r="K9" s="7">
+        <v>5</v>
+      </c>
       <c r="M9">
         <v>4</v>
       </c>
@@ -1234,7 +1238,9 @@
       <c r="J16" s="7">
         <v>5</v>
       </c>
-      <c r="K16" s="6"/>
+      <c r="K16" s="7">
+        <v>5</v>
+      </c>
       <c r="M16" s="10">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_8 декабря 2023 г. 11:23:12_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -579,10 +579,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -950,7 +950,9 @@
       <c r="J10" s="7">
         <v>5</v>
       </c>
-      <c r="K10" s="6"/>
+      <c r="K10" s="7">
+        <v>5</v>
+      </c>
       <c r="M10" s="10">
         <v>3</v>
       </c>
@@ -2034,6 +2036,9 @@
       <c r="I33" s="7">
         <v>5</v>
       </c>
+      <c r="J33" s="7">
+        <v>5</v>
+      </c>
       <c r="K33" s="6"/>
       <c r="M33">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_8 декабря 2023 г. 11:23:41_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -579,10 +579,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
+      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1092,7 +1092,12 @@
       <c r="I13" s="2">
         <v>5</v>
       </c>
-      <c r="K13" s="6"/>
+      <c r="J13" s="10">
+        <v>5</v>
+      </c>
+      <c r="K13" s="10">
+        <v>5</v>
+      </c>
       <c r="M13">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_8 декабря 2023 г. 11:40:45_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -582,7 +582,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
+      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1296,7 +1296,12 @@
       <c r="I17" s="2">
         <v>5</v>
       </c>
-      <c r="K17" s="6"/>
+      <c r="J17" s="10">
+        <v>5</v>
+      </c>
+      <c r="K17" s="10">
+        <v>5</v>
+      </c>
       <c r="M17">
         <v>2</v>
       </c>
@@ -1391,7 +1396,12 @@
       <c r="I19" s="2">
         <v>5</v>
       </c>
-      <c r="K19" s="6"/>
+      <c r="J19" s="7">
+        <v>5</v>
+      </c>
+      <c r="K19" s="7">
+        <v>5</v>
+      </c>
       <c r="M19">
         <v>2</v>
       </c>
@@ -1590,6 +1600,9 @@
       <c r="H23" s="2">
         <v>5</v>
       </c>
+      <c r="I23" s="8">
+        <v>5</v>
+      </c>
       <c r="J23">
         <v>5</v>
       </c>
@@ -1699,7 +1712,9 @@
       <c r="J25" s="8">
         <v>5</v>
       </c>
-      <c r="K25" s="6"/>
+      <c r="K25" s="8">
+        <v>5</v>
+      </c>
       <c r="M25">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_14 декабря 2023 г. 12:29:42_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -569,13 +569,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomRight" activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -587,12 +587,12 @@
     <col min="15" max="18" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
         <v>30</v>
       </c>
@@ -636,7 +636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -663,7 +663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f>IF(B4=C4,1+A3,"____________")</f>
         <v>1</v>
@@ -708,7 +708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A33" si="2">IF(B5=C5,1+A4,"____________")</f>
         <v>2</v>
@@ -740,7 +740,9 @@
       <c r="J5" s="2">
         <v>5</v>
       </c>
-      <c r="L5" s="6"/>
+      <c r="L5" s="8">
+        <v>5</v>
+      </c>
       <c r="N5">
         <v>2</v>
       </c>
@@ -761,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
@@ -812,7 +814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -858,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -916,7 +918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -974,7 +976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -1032,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -1076,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -1134,7 +1136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -1190,7 +1192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -1217,7 +1219,12 @@
       <c r="I14" s="2">
         <v>5</v>
       </c>
-      <c r="L14" s="6"/>
+      <c r="J14" s="8">
+        <v>5</v>
+      </c>
+      <c r="L14" s="10">
+        <v>5</v>
+      </c>
       <c r="N14">
         <v>3</v>
       </c>
@@ -1238,7 +1245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -1295,8 +1302,11 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -1354,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -1404,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -1462,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -1520,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -1552,7 +1562,12 @@
       <c r="J20" s="2">
         <v>5</v>
       </c>
-      <c r="L20" s="6"/>
+      <c r="K20" s="10">
+        <v>5</v>
+      </c>
+      <c r="L20" s="10">
+        <v>5</v>
+      </c>
       <c r="N20">
         <v>2</v>
       </c>
@@ -1573,7 +1588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -1608,7 +1623,9 @@
       <c r="K21" s="7">
         <v>5</v>
       </c>
-      <c r="L21" s="6"/>
+      <c r="L21" s="10">
+        <v>5</v>
+      </c>
       <c r="N21" s="10">
         <v>2</v>
       </c>
@@ -1629,7 +1646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -1683,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -1740,8 +1757,11 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -1799,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -1852,7 +1872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -1903,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -1941,7 +1961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -1978,7 +1998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -2007,7 +2027,15 @@
       <c r="I29" s="2">
         <v>5</v>
       </c>
-      <c r="L29" s="6"/>
+      <c r="K29" s="8">
+        <v>5</v>
+      </c>
+      <c r="L29" s="8">
+        <v>5</v>
+      </c>
+      <c r="M29" s="8">
+        <v>5</v>
+      </c>
       <c r="N29">
         <v>2</v>
       </c>
@@ -2027,8 +2055,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -2078,7 +2109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -2126,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <f t="shared" si="2"/>
         <v>29</v>

</xml_diff>

<commit_message>
AutoCommit_14 декабря 2023 г. 12:33:06_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ДисМат_.xlsx
+++ b/2ИСИП-522_ДисМат_.xlsx
@@ -572,10 +572,10 @@
   <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q5" sqref="Q5"/>
+      <selection pane="bottomRight" activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1666,7 +1666,9 @@
       <c r="F22" s="2">
         <v>5</v>
       </c>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2">
+        <v>5</v>
+      </c>
       <c r="H22" s="2">
         <v>5</v>
       </c>
@@ -1679,7 +1681,12 @@
       <c r="K22">
         <v>5</v>
       </c>
-      <c r="L22" s="6"/>
+      <c r="L22" s="10">
+        <v>5</v>
+      </c>
+      <c r="M22" s="10">
+        <v>5</v>
+      </c>
       <c r="N22">
         <v>1</v>
       </c>

</xml_diff>